<commit_message>
Added another notch filter lol
</commit_message>
<xml_diff>
--- a/Electronics/Filters/Notch/Active TwinT Notch Filter/ExperimentalFrequencyResponseChart.xlsx
+++ b/Electronics/Filters/Notch/Active TwinT Notch Filter/ExperimentalFrequencyResponseChart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Vout</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>dB</t>
+  </si>
+  <si>
+    <t>[</t>
   </si>
 </sst>
 </file>
@@ -648,6 +651,549 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Passive Twin-T Notch Filter Experimental Frequency Response</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ActiveNotchv3!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ActiveNotchv3!$C$24:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ActiveNotchv3!$D$24:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-2.6153656053804761</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.0980391997148637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.349821745875273</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.7314401287412551</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.7448433663685181</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.5250706637687106</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-12.041199826559248</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-14.609741115641675</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-18.416375079047505</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-19.331524890261008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-19.659333214024393</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-14.333975425929008</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-9.1186391129944884</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.0915546130181619</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.7150480853615959</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.0709546997385382</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.31845932194338483</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.12075909994634354</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.390633690625109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7464-4D12-A0F9-9809E3308B77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="409402624"/>
+        <c:axId val="409402952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="409402624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409402952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="409402952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Vout/Vin (dB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409402624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -688,7 +1234,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1237,6 +2339,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC88EE6-C38D-4D68-B46D-4DF62F5319D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1542,10 +2682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D242"/>
+  <dimension ref="A1:R242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1553,7 +2693,7 @@
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1566,8 +2706,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1578,11 +2721,11 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D22" si="0">20*LOG10(B2/A2)</f>
+        <f t="shared" ref="D2:D42" si="0">20*LOG10(B2/A2)</f>
         <v>0.17200343523835138</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1597,7 +2740,7 @@
         <v>8.6427475652851568E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1612,7 +2755,7 @@
         <v>-8.7296108049001758E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1627,7 +2770,7 @@
         <v>-0.72424345308889426</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1642,7 +2785,7 @@
         <v>-1.9382002601611279</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1657,7 +2800,7 @@
         <v>-4.152166210034923</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1672,7 +2815,7 @@
         <v>-8.5425679559903962</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1687,7 +2830,7 @@
         <v>-12.39577516576788</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1702,7 +2845,7 @@
         <v>-15.972057513590968</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1717,7 +2860,7 @@
         <v>-17.393324630099876</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1732,7 +2875,7 @@
         <v>-20.915149811213503</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1747,7 +2890,7 @@
         <v>-19.251470041187527</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1762,7 +2905,7 @@
         <v>-24.013189010928365</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1777,7 +2920,7 @@
         <v>-22.615365605380475</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1792,7 +2935,7 @@
         <v>-14.750978205391412</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1807,7 +2950,7 @@
         <v>-8.7779723270188796</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1822,7 +2965,7 @@
         <v>-4.336226178494849</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1837,7 +2980,7 @@
         <v>-1.4116214857141456</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1851,8 +2994,11 @@
         <f t="shared" si="0"/>
         <v>-0.72424345308889426</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1867,7 +3013,7 @@
         <v>-0.26456531467510319</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1882,85 +3028,311 @@
         <v>8.6427475652851568E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0.5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.6153656053804761</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0.5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="C25" s="1">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.0980391997148637</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0.5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="C26" s="1">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.349821745875273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.5</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C27" s="1">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.7314401287412551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="C28" s="1">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.7448433663685181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.5</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C29" s="1">
+        <v>50</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>-9.5250706637687106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.5</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C30" s="1">
+        <v>55</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>-12.041199826559248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.5</v>
+      </c>
+      <c r="B31" s="1">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>58</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>-14.609741115641675</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.5</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="C32" s="1">
+        <v>60</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>-18.416375079047505</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0.5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>62</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>-19.331524890261008</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>65</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>-19.659333214024393</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0.5</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>70</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>-14.333975425929008</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.5</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C36" s="1">
+        <v>80</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>-9.1186391129944884</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0.5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.221</v>
+      </c>
+      <c r="C37" s="1">
+        <v>90</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.0915546130181619</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.5</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="C38" s="1">
+        <v>100</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.7150480853615959</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0.5</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.442</v>
+      </c>
+      <c r="C39" s="1">
+        <v>150</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.0709546997385382</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0.5</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="C40" s="1">
+        <v>200</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.31845932194338483</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0.5</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="C41" s="1">
+        <v>300</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12075909994634354</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0.5</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="C42" s="1">
+        <v>500</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.390633690625109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>